<commit_message>
Letters lists are sorted too
</commit_message>
<xml_diff>
--- a/cp1/kozak_fb-12_vysotskyi_fb-12_cp1/data.xlsx
+++ b/cp1/kozak_fb-12_vysotskyi_fb-12_cp1/data.xlsx
@@ -12,6 +12,7 @@
   </sheets>
   <definedNames>
     <definedName name="data" localSheetId="0">Лист2!$A$2:$AI$216</definedName>
+    <definedName name="ExternalData_1" localSheetId="0">Лист2!$A$37:$B$69</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
@@ -19,7 +20,15 @@
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <connection id="1" name="data1" type="6" refreshedVersion="4" background="1" saveData="1">
+  <connection id="1" name="data" type="6" refreshedVersion="4" background="1" saveData="1">
+    <textPr codePage="65001" sourceFile="D:\Maksym\Crypt\crypto-23-24\cp1\kozak_fb-12_vysotskyi_fb-12_cp1\data.csv" decimal="," thousands=" " tab="0" space="1" comma="1" semicolon="1" consecutive="1">
+      <textFields count="2">
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="2" name="data1" type="6" refreshedVersion="4" background="1" saveData="1">
     <textPr codePage="65001" sourceFile="D:\Maksym\Crypt\crypto-23-24\cp1\kozak_fb-12_vysotskyi_fb-12_cp1\data.csv" decimal="," thousands=" " tab="0" space="1" comma="1" consecutive="1">
       <textFields count="2">
         <textField/>
@@ -31,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3901" uniqueCount="289">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3900" uniqueCount="288">
   <si>
     <t>н</t>
   </si>
@@ -895,9 +904,6 @@
   </si>
   <si>
     <t>Частоти біграм з перетинами з пробілами</t>
-  </si>
-  <si>
-    <t>_</t>
   </si>
 </sst>
 </file>
@@ -961,7 +967,11 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="data" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="ExternalData_1" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="data" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1253,8 +1263,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AI211"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A196" workbookViewId="0">
-      <selection activeCell="M183" sqref="M183"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F44" sqref="F44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1289,75 +1299,72 @@
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
       <c r="B2" t="s">
-        <v>1</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="B4" t="s">
-        <v>5</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="B5" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="B6" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="B7" t="s">
-        <v>11</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>12</v>
+        <v>39</v>
       </c>
       <c r="B8" t="s">
-        <v>13</v>
+        <v>40</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>288</v>
+        <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="B10" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
@@ -1370,122 +1377,122 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="B12" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>21</v>
+        <v>4</v>
       </c>
       <c r="B13" t="s">
-        <v>22</v>
+        <v>5</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>23</v>
+        <v>47</v>
       </c>
       <c r="B14" t="s">
-        <v>24</v>
+        <v>48</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="B15" t="s">
-        <v>26</v>
+        <v>36</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>27</v>
+        <v>37</v>
       </c>
       <c r="B16" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="B17" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>31</v>
+        <v>41</v>
       </c>
       <c r="B18" t="s">
-        <v>32</v>
+        <v>42</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B19" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>35</v>
+        <v>55</v>
       </c>
       <c r="B20" t="s">
-        <v>36</v>
+        <v>56</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="B21" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>39</v>
+        <v>53</v>
       </c>
       <c r="B22" t="s">
-        <v>40</v>
+        <v>54</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="B23" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>43</v>
+        <v>19</v>
       </c>
       <c r="B24" t="s">
-        <v>44</v>
+        <v>20</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="B25" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>47</v>
+        <v>12</v>
       </c>
       <c r="B26" t="s">
-        <v>48</v>
+        <v>13</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
@@ -1498,58 +1505,58 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="B28" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>53</v>
+        <v>27</v>
       </c>
       <c r="B29" t="s">
-        <v>54</v>
+        <v>28</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="B30" t="s">
-        <v>56</v>
+        <v>62</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="B31" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B32" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="B33" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="B34" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.3">
@@ -1579,66 +1586,66 @@
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="B37" t="s">
-        <v>3</v>
+        <v>69</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="B38" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="B39" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B40" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="B41" t="s">
-        <v>70</v>
+        <v>3</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>10</v>
+        <v>39</v>
       </c>
       <c r="B42" t="s">
-        <v>71</v>
+        <v>83</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B43" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="B44" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.3">
@@ -1651,122 +1658,122 @@
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="B46" t="s">
-        <v>34</v>
+        <v>76</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>21</v>
+        <v>4</v>
       </c>
       <c r="B47" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>23</v>
+        <v>47</v>
       </c>
       <c r="B48" t="s">
-        <v>75</v>
+        <v>87</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="B49" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>27</v>
+        <v>37</v>
       </c>
       <c r="B50" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="B51" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>31</v>
+        <v>41</v>
       </c>
       <c r="B52" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B53" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>35</v>
+        <v>55</v>
       </c>
       <c r="B54" t="s">
-        <v>81</v>
+        <v>90</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="B55" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>39</v>
+        <v>53</v>
       </c>
       <c r="B56" t="s">
-        <v>83</v>
+        <v>89</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="B57" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>43</v>
+        <v>19</v>
       </c>
       <c r="B58" t="s">
-        <v>85</v>
+        <v>34</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="B59" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>47</v>
+        <v>12</v>
       </c>
       <c r="B60" t="s">
-        <v>87</v>
+        <v>72</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.3">
@@ -1779,58 +1786,58 @@
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="B62" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>53</v>
+        <v>27</v>
       </c>
       <c r="B63" t="s">
-        <v>89</v>
+        <v>77</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="B64" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
     </row>
     <row r="65" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="B65" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
     </row>
     <row r="66" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B66" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="67" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="B67" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="68" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="B68" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="69" spans="1:35" x14ac:dyDescent="0.3">
@@ -16480,9 +16487,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A38" workbookViewId="0">
+      <selection activeCell="A35" sqref="A35:B67"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="2.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.5546875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Fixed incorrect H2 calculation
</commit_message>
<xml_diff>
--- a/cp1/kozak_fb-12_vysotskyi_fb-12_cp1/data.xlsx
+++ b/cp1/kozak_fb-12_vysotskyi_fb-12_cp1/data.xlsx
@@ -1263,8 +1263,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AI211"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F44" sqref="F44"/>
+    <sheetView tabSelected="1" topLeftCell="A158" workbookViewId="0">
+      <selection activeCell="J177" sqref="J177"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1856,7 +1856,7 @@
         <v>281</v>
       </c>
       <c r="G70" s="2">
-        <v>7.9008500000000002</v>
+        <v>3.9504299999999999</v>
       </c>
       <c r="H70" s="1" t="s">
         <v>282</v>
@@ -5618,7 +5618,7 @@
         <v>281</v>
       </c>
       <c r="G106" s="2">
-        <v>7.8997799999999998</v>
+        <v>3.9498899999999999</v>
       </c>
       <c r="H106" s="1" t="s">
         <v>282</v>
@@ -9380,7 +9380,7 @@
         <v>281</v>
       </c>
       <c r="G142" s="2">
-        <v>8.2591999999999999</v>
+        <v>4.1295999999999999</v>
       </c>
       <c r="H142" s="1" t="s">
         <v>282</v>
@@ -12933,7 +12933,7 @@
         <v>281</v>
       </c>
       <c r="G177" s="2">
-        <v>8.2576400000000003</v>
+        <v>4.1288200000000002</v>
       </c>
       <c r="H177" s="1" t="s">
         <v>282</v>

</xml_diff>